<commit_message>
added errors per tester
</commit_message>
<xml_diff>
--- a/Evaluation/ergebnisse/ergebnisse.xlsx
+++ b/Evaluation/ergebnisse/ergebnisse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annas\Documents\Uni\3Semester\MobileGISAnwendungen\Ue\BankoMap\Evaluation\ergebnisse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danabe00\Desktop\geodaesie\Semester 9\mobile GIS anwendungen\BankoMap\BankoMap\Evaluation\ergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74693AA-67DA-42F1-96F2-31B793AD1D4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8303BD8-6E70-4345-91AE-09802EBB60D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{329184E2-A708-4ACE-9A57-C234AC1F08F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="7" xr2:uid="{329184E2-A708-4ACE-9A57-C234AC1F08F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,22 +22,17 @@
     <sheet name="Tabelle7" sheetId="7" r:id="rId7"/>
     <sheet name="Tabelle8" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -200,7 +195,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -267,15 +262,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -293,7 +288,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -330,7 +325,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -519,7 +514,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -557,7 +552,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564800504"/>
@@ -636,7 +631,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -674,7 +669,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564803784"/>
@@ -722,7 +717,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -736,7 +731,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -798,7 +793,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -984,7 +979,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1022,7 +1017,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564824776"/>
@@ -1101,7 +1096,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1139,7 +1134,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564824120"/>
@@ -1187,7 +1182,7 @@
       <a:pPr>
         <a:defRPr sz="900"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1201,7 +1196,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1263,7 +1258,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1448,7 +1443,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1486,7 +1481,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="615406976"/>
@@ -1570,7 +1565,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1608,7 +1603,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="615396152"/>
@@ -1656,7 +1651,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3449,7 +3444,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3748,10 +3743,10 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4138,11 +4133,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0DB85F-ED90-44B2-830D-FB96ACDEAF4C}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -4443,7 +4438,7 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -4747,7 +4742,7 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5048,7 +5043,7 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5346,10 +5341,10 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5650,7 +5645,7 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -5950,11 +5945,11 @@
   </sheetPr>
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5546875" bestFit="1" customWidth="1"/>
@@ -6042,7 +6037,9 @@
       <c r="J3" s="1">
         <v>2</v>
       </c>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
@@ -6076,7 +6073,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6110,7 +6107,9 @@
       <c r="J5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
@@ -6209,6 +6208,9 @@
       <c r="J10" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="K10" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
@@ -6241,7 +6243,9 @@
       <c r="J11" s="1">
         <v>1</v>
       </c>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -6275,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="K12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6309,7 +6313,9 @@
       <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="K13" s="1"/>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
@@ -6342,7 +6348,9 @@
       <c r="J14" s="1">
         <v>3</v>
       </c>
-      <c r="K14" s="1"/>
+      <c r="K14" s="1">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">

</xml_diff>